<commit_message>
Updated to Version 1.3
Added TS ID´s and Priorities.
</commit_message>
<xml_diff>
--- a/test_cases/TC-01.xlsx
+++ b/test_cases/TC-01.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="124">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -94,10 +94,19 @@
     <t>State = Houston</t>
   </si>
   <si>
-    <t>Postal Code = 1234</t>
-  </si>
-  <si>
-    <t>Phone = +48512354</t>
+    <t>Postal Code = 77001</t>
+  </si>
+  <si>
+    <t>Phone = +148512354</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>TS-1A</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
   <si>
     <t>Test Scenario</t>
@@ -250,6 +259,12 @@
     <t>The State field should be filled</t>
   </si>
   <si>
+    <t>User inputs his Zip Code</t>
+  </si>
+  <si>
+    <t>The Zip Code field should be filled</t>
+  </si>
+  <si>
     <t>User inputs his Phone number</t>
   </si>
   <si>
@@ -280,6 +295,9 @@
     <t>DoB = 15/08/1990</t>
   </si>
   <si>
+    <t>TS-1B</t>
+  </si>
+  <si>
     <t>Company = Harasaka Motors</t>
   </si>
   <si>
@@ -301,7 +319,7 @@
     <t>Postal Code = 10012</t>
   </si>
   <si>
-    <t>Phone = +4874523</t>
+    <t>Phone = +14234848</t>
   </si>
   <si>
     <r>
@@ -364,6 +382,12 @@
     <t>DoB = 20/01/1895</t>
   </si>
   <si>
+    <t>TS-1C</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
     <t>Company = Müller Electronics</t>
   </si>
   <si>
@@ -399,6 +423,12 @@
   <si>
     <t xml:space="preserve">The Password field should be filled </t>
   </si>
+  <si>
+    <t>User inputs her Address</t>
+  </si>
+  <si>
+    <t>The Zip Code field should be filled  but be shown as invalid</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +437,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d.m"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -437,6 +467,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -510,7 +545,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +556,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
@@ -773,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -849,10 +890,19 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -861,12 +911,12 @@
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="18" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -875,34 +925,34 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="21" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -914,25 +964,31 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -941,6 +997,9 @@
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1216,7 +1275,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="14">
-        <v>44562.0</v>
+        <v>44593.0</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -1264,7 +1323,7 @@
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" ht="30.75" customHeight="1">
       <c r="D6" s="21">
         <v>1.0</v>
       </c>
@@ -1383,558 +1442,584 @@
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="A20" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="15"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
-      <c r="G21" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="37"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="G21" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="40"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="41" t="s">
+      <c r="A22" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="B22" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="42" t="s">
+      <c r="C22" s="43"/>
+      <c r="D22" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="37"/>
-      <c r="K22" s="42" t="s">
+      <c r="E22" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L22" s="37"/>
-      <c r="M22" s="42" t="s">
+      <c r="G22" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="37"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="40"/>
+      <c r="K22" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="40"/>
+      <c r="M22" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="40"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="G23" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="37"/>
-      <c r="K23" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="L23" s="37"/>
-      <c r="M23" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="N23" s="37"/>
+      <c r="G23" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="40"/>
+      <c r="I23" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="40"/>
+      <c r="K23" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="40"/>
+      <c r="M23" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="40"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>44</v>
+      <c r="A24" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="46" t="s">
-        <v>45</v>
+      <c r="D24" s="49" t="s">
+        <v>48</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="G24" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="K24" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="M24" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="N24" s="47" t="s">
-        <v>47</v>
+      <c r="G24" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="N24" s="50" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="48">
+      <c r="A25" s="51">
         <v>1.0</v>
       </c>
-      <c r="B25" s="49" t="s">
-        <v>48</v>
+      <c r="B25" s="52" t="s">
+        <v>51</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="50" t="s">
-        <v>49</v>
+      <c r="D25" s="53" t="s">
+        <v>52</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="G25" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J25" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L25" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" s="51"/>
-      <c r="N25" s="52" t="s">
-        <v>53</v>
+      <c r="G25" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M25" s="54"/>
+      <c r="N25" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="25.5" customHeight="1">
-      <c r="A26" s="48">
+      <c r="A26" s="51">
         <v>2.0</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>54</v>
+      <c r="B26" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="C26" s="6"/>
-      <c r="D26" s="54" t="s">
-        <v>55</v>
+      <c r="D26" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="E26" s="6"/>
-      <c r="G26" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I26" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L26" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M26" s="51"/>
-      <c r="N26" s="52" t="s">
-        <v>53</v>
+      <c r="G26" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M26" s="54"/>
+      <c r="N26" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" ht="25.5" customHeight="1">
-      <c r="A27" s="48">
+      <c r="A27" s="51">
         <v>3.0</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="G27" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="G27" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="K27" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M27" s="51"/>
-      <c r="N27" s="52" t="s">
-        <v>53</v>
+      <c r="K27" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M27" s="54"/>
+      <c r="N27" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" ht="25.5" customHeight="1">
-      <c r="A28" s="48">
+      <c r="A28" s="51">
         <v>4.0</v>
       </c>
-      <c r="B28" s="54" t="s">
-        <v>58</v>
+      <c r="B28" s="57" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="54" t="s">
-        <v>59</v>
+      <c r="D28" s="57" t="s">
+        <v>62</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="G28" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="K28" s="55"/>
+      <c r="G28" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="58"/>
       <c r="L28" s="25"/>
-      <c r="M28" s="55"/>
+      <c r="M28" s="58"/>
       <c r="N28" s="25"/>
     </row>
     <row r="29" ht="25.5" customHeight="1">
-      <c r="A29" s="56">
+      <c r="A29" s="59">
         <v>5.0</v>
       </c>
-      <c r="B29" s="54" t="s">
-        <v>60</v>
+      <c r="B29" s="57" t="s">
+        <v>63</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="54" t="s">
-        <v>61</v>
+      <c r="D29" s="57" t="s">
+        <v>64</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="G29" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" s="55"/>
+      <c r="G29" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="58"/>
       <c r="L29" s="25"/>
-      <c r="M29" s="55"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="25"/>
     </row>
     <row r="30" ht="25.5" customHeight="1">
-      <c r="A30" s="56">
+      <c r="A30" s="59">
         <v>6.0</v>
       </c>
-      <c r="B30" s="54" t="s">
-        <v>62</v>
+      <c r="B30" s="57" t="s">
+        <v>65</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="54" t="s">
-        <v>63</v>
+      <c r="D30" s="57" t="s">
+        <v>66</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="G30" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J30" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="K30" s="55"/>
+      <c r="G30" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="58"/>
       <c r="L30" s="25"/>
-      <c r="M30" s="55"/>
+      <c r="M30" s="58"/>
       <c r="N30" s="25"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="56">
+      <c r="A31" s="59">
         <v>7.0</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>64</v>
+      <c r="B31" s="57" t="s">
+        <v>67</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="D31" s="54" t="s">
-        <v>65</v>
+      <c r="D31" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="E31" s="6"/>
-      <c r="G31" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I31" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J31" s="52" t="s">
-        <v>53</v>
+      <c r="G31" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="56">
+      <c r="A32" s="59">
         <v>8.0</v>
       </c>
-      <c r="B32" s="54" t="s">
-        <v>66</v>
+      <c r="B32" s="57" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="54" t="s">
-        <v>67</v>
+      <c r="D32" s="57" t="s">
+        <v>70</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="G32" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H32" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J32" s="52" t="s">
-        <v>53</v>
+      <c r="G32" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="56">
+      <c r="A33" s="59">
         <v>9.0</v>
       </c>
-      <c r="B33" s="54" t="s">
-        <v>68</v>
+      <c r="B33" s="57" t="s">
+        <v>71</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="54" t="s">
-        <v>69</v>
+      <c r="D33" s="57" t="s">
+        <v>72</v>
       </c>
       <c r="E33" s="6"/>
-      <c r="G33" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I33" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="52" t="s">
-        <v>53</v>
+      <c r="G33" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J33" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="56">
+      <c r="A34" s="59">
         <v>10.0</v>
       </c>
-      <c r="B34" s="54" t="s">
-        <v>70</v>
+      <c r="B34" s="57" t="s">
+        <v>73</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="54" t="s">
-        <v>71</v>
+      <c r="D34" s="57" t="s">
+        <v>74</v>
       </c>
       <c r="E34" s="6"/>
-      <c r="G34" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I34" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J34" s="52" t="s">
-        <v>53</v>
+      <c r="G34" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="56">
+      <c r="A35" s="59">
         <v>11.0</v>
       </c>
-      <c r="B35" s="54" t="s">
-        <v>72</v>
+      <c r="B35" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="C35" s="6"/>
-      <c r="D35" s="54" t="s">
-        <v>73</v>
+      <c r="D35" s="57" t="s">
+        <v>76</v>
       </c>
       <c r="E35" s="6"/>
-      <c r="G35" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I35" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="52" t="s">
-        <v>53</v>
+      <c r="G35" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H35" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="56">
+      <c r="A36" s="59">
         <v>12.0</v>
       </c>
-      <c r="B36" s="54" t="s">
-        <v>74</v>
+      <c r="B36" s="57" t="s">
+        <v>77</v>
       </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="54" t="s">
-        <v>75</v>
+      <c r="D36" s="57" t="s">
+        <v>78</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="G36" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H36" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I36" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J36" s="52" t="s">
-        <v>53</v>
+      <c r="G36" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="55" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="56">
+      <c r="A37" s="59">
         <v>13.0</v>
       </c>
-      <c r="B37" s="54" t="s">
-        <v>76</v>
+      <c r="B37" s="57" t="s">
+        <v>79</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="D37" s="54" t="s">
-        <v>77</v>
+      <c r="D37" s="57" t="s">
+        <v>80</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="G37" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H37" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I37" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1"/>
+      <c r="G37" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J37" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="59">
+        <v>14.0</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="6"/>
+    </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="G39" s="57" t="s">
-        <v>78</v>
+      <c r="G39" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="57" t="s">
-        <v>78</v>
+      <c r="I39" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="J39" s="6"/>
-      <c r="K39" s="57" t="s">
-        <v>78</v>
+      <c r="K39" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="L39" s="6"/>
-      <c r="M39" s="57" t="s">
-        <v>78</v>
+      <c r="M39" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="N39" s="6"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="G40" s="58"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="59" t="s">
-        <v>79</v>
+      <c r="I40" s="62" t="s">
+        <v>84</v>
       </c>
       <c r="J40" s="6"/>
-      <c r="K40" s="58"/>
+      <c r="K40" s="61"/>
       <c r="L40" s="6"/>
-      <c r="M40" s="58"/>
+      <c r="M40" s="61"/>
       <c r="N40" s="6"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="G41" s="58"/>
+      <c r="G41" s="61"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="58"/>
+      <c r="I41" s="61"/>
       <c r="J41" s="6"/>
-      <c r="K41" s="58"/>
+      <c r="K41" s="61"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="58"/>
+      <c r="M41" s="61"/>
       <c r="N41" s="6"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="G42" s="58"/>
+      <c r="G42" s="61"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="58"/>
+      <c r="I42" s="61"/>
       <c r="J42" s="6"/>
-      <c r="K42" s="58"/>
+      <c r="K42" s="61"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="58"/>
+      <c r="M42" s="61"/>
       <c r="N42" s="6"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="G43" s="58"/>
+      <c r="G43" s="61"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="58"/>
+      <c r="I43" s="61"/>
       <c r="J43" s="6"/>
-      <c r="K43" s="58"/>
+      <c r="K43" s="61"/>
       <c r="L43" s="6"/>
-      <c r="M43" s="58"/>
+      <c r="M43" s="61"/>
       <c r="N43" s="6"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="G44" s="58"/>
+      <c r="G44" s="61"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="58"/>
+      <c r="I44" s="61"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="58"/>
+      <c r="K44" s="61"/>
       <c r="L44" s="6"/>
-      <c r="M44" s="58"/>
+      <c r="M44" s="61"/>
       <c r="N44" s="6"/>
     </row>
     <row r="45" ht="14.25" customHeight="1"/>
@@ -1962,7 +2047,7 @@
         <v>2.0</v>
       </c>
       <c r="K51" s="22" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
@@ -1970,7 +2055,7 @@
         <v>3.0</v>
       </c>
       <c r="K52" s="22" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1978,7 +2063,7 @@
         <v>4.0</v>
       </c>
       <c r="K53" s="22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
@@ -1986,28 +2071,41 @@
         <v>5.0</v>
       </c>
       <c r="K54" s="22" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="6"/>
       <c r="J55" s="26">
         <v>6.0</v>
       </c>
       <c r="K55" s="22" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="30"/>
-      <c r="G56" s="61" t="s">
+      <c r="A56" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
+      <c r="G56" s="66" t="s">
         <v>12</v>
       </c>
       <c r="H56" s="13" t="s">
@@ -2017,13 +2115,13 @@
         <v>7.0</v>
       </c>
       <c r="K56" s="22" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="62"/>
-      <c r="B57" s="63"/>
-      <c r="E57" s="64"/>
+      <c r="A57" s="67"/>
+      <c r="B57" s="68"/>
+      <c r="E57" s="69"/>
       <c r="G57" s="24">
         <v>1.0</v>
       </c>
@@ -2034,15 +2132,15 @@
         <v>8.0</v>
       </c>
       <c r="K57" s="22" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="37"/>
       <c r="G58" s="24">
         <v>2.0</v>
       </c>
@@ -2053,22 +2151,22 @@
         <v>9.0</v>
       </c>
       <c r="K58" s="22" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B59" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="40"/>
-      <c r="D59" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="41" t="s">
+      <c r="A59" s="41" t="s">
         <v>35</v>
+      </c>
+      <c r="B59" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="43"/>
+      <c r="D59" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="G59" s="24">
         <v>3.0</v>
@@ -2078,7 +2176,7 @@
         <v>10.0</v>
       </c>
       <c r="K59" s="22" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
@@ -2090,534 +2188,545 @@
         <v>11.0</v>
       </c>
       <c r="K60" s="22" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1"/>
     <row r="62" ht="14.25" customHeight="1"/>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="G63" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="39"/>
+      <c r="N63" s="40"/>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="51">
+        <v>1.0</v>
+      </c>
+      <c r="B64" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="G64" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H64" s="40"/>
+      <c r="I64" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J64" s="40"/>
+      <c r="K64" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="L64" s="40"/>
+      <c r="M64" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="N64" s="40"/>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="51">
+        <v>2.0</v>
+      </c>
+      <c r="B65" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="G65" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="H65" s="40"/>
+      <c r="I65" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="46" t="s">
+      <c r="J65" s="40"/>
+      <c r="K65" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="L65" s="40"/>
+      <c r="M65" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="6"/>
-      <c r="G63" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H63" s="36"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="36"/>
-      <c r="K63" s="36"/>
-      <c r="L63" s="36"/>
-      <c r="M63" s="36"/>
-      <c r="N63" s="37"/>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="48">
-        <v>1.0</v>
-      </c>
-      <c r="B64" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="50" t="s">
+      <c r="N65" s="40"/>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="51">
+        <v>3.0</v>
+      </c>
+      <c r="B66" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="G66" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E64" s="6"/>
-      <c r="G64" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H64" s="37"/>
-      <c r="I64" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="J64" s="37"/>
-      <c r="K64" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="L64" s="37"/>
-      <c r="M64" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="N64" s="37"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="48">
-        <v>2.0</v>
-      </c>
-      <c r="B65" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="54" t="s">
+      <c r="H66" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I66" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="J66" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="K66" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="L66" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="M66" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="N66" s="50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="51">
+        <v>4.0</v>
+      </c>
+      <c r="B67" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" s="6"/>
+      <c r="G67" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H67" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I67" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J67" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K67" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L67" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M67" s="54"/>
+      <c r="N67" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" s="59">
+        <v>5.0</v>
+      </c>
+      <c r="B68" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="G68" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H68" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I68" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J68" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K68" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L68" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M68" s="54"/>
+      <c r="N68" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" s="59">
+        <v>6.0</v>
+      </c>
+      <c r="B69" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="E69" s="6"/>
+      <c r="G69" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H69" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J69" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K69" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L69" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M69" s="54"/>
+      <c r="N69" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" s="59">
+        <v>7.0</v>
+      </c>
+      <c r="B70" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" s="6"/>
+      <c r="G70" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H70" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I70" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J70" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K70" s="58"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="25"/>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="59">
+        <v>8.0</v>
+      </c>
+      <c r="B71" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" s="6"/>
+      <c r="G71" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H71" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J71" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K71" s="58"/>
+      <c r="L71" s="25"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="25"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="59">
+        <v>9.0</v>
+      </c>
+      <c r="B72" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E72" s="6"/>
+      <c r="G72" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H72" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I72" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J72" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E65" s="6"/>
-      <c r="G65" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H65" s="37"/>
-      <c r="I65" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="J65" s="37"/>
-      <c r="K65" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="L65" s="37"/>
-      <c r="M65" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="N65" s="37"/>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="48">
-        <v>3.0</v>
-      </c>
-      <c r="B66" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E66" s="6"/>
-      <c r="G66" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="I66" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J66" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="K66" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="L66" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="M66" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="N66" s="47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="48">
-        <v>4.0</v>
-      </c>
-      <c r="B67" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="E67" s="6"/>
-      <c r="G67" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H67" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I67" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J67" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K67" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L67" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M67" s="51"/>
-      <c r="N67" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="56">
-        <v>5.0</v>
-      </c>
-      <c r="B68" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="E68" s="6"/>
-      <c r="G68" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H68" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I68" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J68" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K68" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L68" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M68" s="51"/>
-      <c r="N68" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="56">
-        <v>6.0</v>
-      </c>
-      <c r="B69" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="6"/>
-      <c r="G69" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H69" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I69" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J69" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K69" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L69" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M69" s="51"/>
-      <c r="N69" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="56">
-        <v>7.0</v>
-      </c>
-      <c r="B70" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="G70" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H70" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I70" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J70" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K70" s="55"/>
-      <c r="L70" s="25"/>
-      <c r="M70" s="55"/>
-      <c r="N70" s="25"/>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="56">
-        <v>8.0</v>
-      </c>
-      <c r="B71" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E71" s="6"/>
-      <c r="G71" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H71" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I71" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J71" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K71" s="55"/>
-      <c r="L71" s="25"/>
-      <c r="M71" s="55"/>
-      <c r="N71" s="25"/>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="56">
-        <v>9.0</v>
-      </c>
-      <c r="B72" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E72" s="6"/>
-      <c r="G72" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H72" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I72" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J72" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="K72" s="55"/>
+      <c r="K72" s="58"/>
       <c r="L72" s="25"/>
-      <c r="M72" s="55"/>
+      <c r="M72" s="58"/>
       <c r="N72" s="25"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="56">
+      <c r="A73" s="59">
         <v>10.0</v>
       </c>
-      <c r="B73" s="54" t="s">
-        <v>97</v>
+      <c r="B73" s="57" t="s">
+        <v>103</v>
       </c>
       <c r="C73" s="6"/>
-      <c r="D73" s="54" t="s">
-        <v>71</v>
+      <c r="D73" s="57" t="s">
+        <v>74</v>
       </c>
       <c r="E73" s="6"/>
-      <c r="G73" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H73" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I73" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J73" s="52" t="s">
-        <v>51</v>
+      <c r="G73" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H73" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I73" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J73" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="56">
+      <c r="A74" s="59">
         <v>11.0</v>
       </c>
-      <c r="B74" s="54" t="s">
-        <v>98</v>
+      <c r="B74" s="57" t="s">
+        <v>104</v>
       </c>
       <c r="C74" s="6"/>
-      <c r="D74" s="54" t="s">
-        <v>73</v>
+      <c r="D74" s="57" t="s">
+        <v>76</v>
       </c>
       <c r="E74" s="6"/>
-      <c r="G74" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H74" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I74" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J74" s="52" t="s">
-        <v>51</v>
+      <c r="G74" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H74" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I74" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J74" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="56">
+      <c r="A75" s="59">
         <v>12.0</v>
       </c>
-      <c r="B75" s="54" t="s">
-        <v>99</v>
+      <c r="B75" s="57" t="s">
+        <v>77</v>
       </c>
       <c r="C75" s="6"/>
-      <c r="D75" s="54" t="s">
-        <v>75</v>
+      <c r="D75" s="57" t="s">
+        <v>78</v>
       </c>
       <c r="E75" s="6"/>
-      <c r="G75" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H75" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I75" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J75" s="52" t="s">
-        <v>51</v>
+      <c r="G75" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H75" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I75" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J75" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="56">
+      <c r="A76" s="59">
         <v>13.0</v>
       </c>
-      <c r="B76" s="54" t="s">
-        <v>76</v>
+      <c r="B76" s="57" t="s">
+        <v>105</v>
       </c>
       <c r="C76" s="6"/>
-      <c r="D76" s="54" t="s">
-        <v>100</v>
+      <c r="D76" s="57" t="s">
+        <v>80</v>
       </c>
       <c r="E76" s="6"/>
-      <c r="G76" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H76" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I76" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J76" s="52" t="s">
-        <v>51</v>
+      <c r="G76" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H76" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I76" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J76" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="G77" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H77" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I77" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J77" s="52" t="s">
-        <v>51</v>
+      <c r="A77" s="59">
+        <v>14.0</v>
+      </c>
+      <c r="B77" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" s="6"/>
+      <c r="G77" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H77" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I77" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J77" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="G78" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H78" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I78" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J78" s="52" t="s">
-        <v>51</v>
+      <c r="G78" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H78" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I78" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J78" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="G79" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H79" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I79" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J79" s="53" t="s">
-        <v>52</v>
+      <c r="G79" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H79" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I79" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J79" s="56" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="G81" s="57" t="s">
-        <v>78</v>
+      <c r="G81" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="H81" s="6"/>
-      <c r="I81" s="57" t="s">
-        <v>78</v>
+      <c r="I81" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="J81" s="6"/>
-      <c r="K81" s="57" t="s">
-        <v>78</v>
+      <c r="K81" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="L81" s="6"/>
-      <c r="M81" s="57" t="s">
-        <v>78</v>
+      <c r="M81" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="N81" s="6"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="G82" s="58"/>
+      <c r="G82" s="61"/>
       <c r="H82" s="6"/>
-      <c r="I82" s="59" t="s">
-        <v>101</v>
+      <c r="I82" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="J82" s="6"/>
-      <c r="K82" s="58"/>
+      <c r="K82" s="61"/>
       <c r="L82" s="6"/>
-      <c r="M82" s="58"/>
+      <c r="M82" s="61"/>
       <c r="N82" s="6"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="G83" s="58"/>
+      <c r="G83" s="61"/>
       <c r="H83" s="6"/>
-      <c r="I83" s="59" t="s">
-        <v>102</v>
+      <c r="I83" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="J83" s="6"/>
-      <c r="K83" s="58"/>
+      <c r="K83" s="61"/>
       <c r="L83" s="6"/>
-      <c r="M83" s="58"/>
+      <c r="M83" s="61"/>
       <c r="N83" s="6"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="G84" s="58"/>
+      <c r="G84" s="61"/>
       <c r="H84" s="6"/>
-      <c r="I84" s="58"/>
+      <c r="I84" s="61"/>
       <c r="J84" s="6"/>
-      <c r="K84" s="58"/>
+      <c r="K84" s="61"/>
       <c r="L84" s="6"/>
-      <c r="M84" s="58"/>
+      <c r="M84" s="61"/>
       <c r="N84" s="6"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="G85" s="58"/>
+      <c r="G85" s="61"/>
       <c r="H85" s="6"/>
-      <c r="I85" s="58"/>
+      <c r="I85" s="61"/>
       <c r="J85" s="6"/>
-      <c r="K85" s="58"/>
+      <c r="K85" s="61"/>
       <c r="L85" s="6"/>
-      <c r="M85" s="58"/>
+      <c r="M85" s="61"/>
       <c r="N85" s="6"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="G86" s="58"/>
+      <c r="G86" s="61"/>
       <c r="H86" s="6"/>
-      <c r="I86" s="58"/>
+      <c r="I86" s="61"/>
       <c r="J86" s="6"/>
-      <c r="K86" s="58"/>
+      <c r="K86" s="61"/>
       <c r="L86" s="6"/>
-      <c r="M86" s="58"/>
+      <c r="M86" s="61"/>
       <c r="N86" s="6"/>
     </row>
     <row r="87" ht="14.25" customHeight="1"/>
@@ -2642,7 +2751,7 @@
         <v>2.0</v>
       </c>
       <c r="K90" s="22" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
@@ -2650,7 +2759,7 @@
         <v>3.0</v>
       </c>
       <c r="K91" s="22" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -2658,7 +2767,7 @@
         <v>4.0</v>
       </c>
       <c r="K92" s="22" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
@@ -2666,28 +2775,41 @@
         <v>5.0</v>
       </c>
       <c r="K93" s="22" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
+      <c r="A94" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C94" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="E94" s="6"/>
       <c r="J94" s="26">
         <v>6.0</v>
       </c>
       <c r="K94" s="22" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B95" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="30"/>
-      <c r="G95" s="61" t="s">
+      <c r="A95" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B95" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="33"/>
+      <c r="G95" s="66" t="s">
         <v>12</v>
       </c>
       <c r="H95" s="13" t="s">
@@ -2697,13 +2819,13 @@
         <v>7.0</v>
       </c>
       <c r="K95" s="22" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="62"/>
-      <c r="B96" s="63"/>
-      <c r="E96" s="64"/>
+      <c r="A96" s="67"/>
+      <c r="B96" s="68"/>
+      <c r="E96" s="69"/>
       <c r="G96" s="24">
         <v>1.0</v>
       </c>
@@ -2714,15 +2836,15 @@
         <v>8.0</v>
       </c>
       <c r="K96" s="22" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="31"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="33"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="34"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="37"/>
       <c r="G97" s="24">
         <v>2.0</v>
       </c>
@@ -2733,22 +2855,22 @@
         <v>9.0</v>
       </c>
       <c r="K97" s="22" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B98" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C98" s="40"/>
-      <c r="D98" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E98" s="41" t="s">
+      <c r="A98" s="41" t="s">
         <v>35</v>
+      </c>
+      <c r="B98" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" s="43"/>
+      <c r="D98" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E98" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="G98" s="24">
         <v>3.0</v>
@@ -2758,7 +2880,7 @@
         <v>10.0</v>
       </c>
       <c r="K98" s="22" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
@@ -2770,534 +2892,545 @@
         <v>11.0</v>
       </c>
       <c r="K99" s="22" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1"/>
     <row r="101" ht="14.25" customHeight="1"/>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="44" t="s">
+      <c r="A102" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E102" s="6"/>
+      <c r="G102" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H102" s="39"/>
+      <c r="I102" s="39"/>
+      <c r="J102" s="39"/>
+      <c r="K102" s="39"/>
+      <c r="L102" s="39"/>
+      <c r="M102" s="39"/>
+      <c r="N102" s="40"/>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="A103" s="51">
+        <v>1.0</v>
+      </c>
+      <c r="B103" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C103" s="6"/>
+      <c r="D103" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="6"/>
+      <c r="G103" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H103" s="40"/>
+      <c r="I103" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J103" s="40"/>
+      <c r="K103" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="L103" s="40"/>
+      <c r="M103" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="N103" s="40"/>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="A104" s="51">
+        <v>2.0</v>
+      </c>
+      <c r="B104" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C104" s="6"/>
+      <c r="D104" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E104" s="6"/>
+      <c r="G104" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B102" s="45" t="s">
+      <c r="H104" s="40"/>
+      <c r="I104" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="46" t="s">
+      <c r="J104" s="40"/>
+      <c r="K104" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="L104" s="40"/>
+      <c r="M104" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="E102" s="6"/>
-      <c r="G102" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
-      <c r="K102" s="36"/>
-      <c r="L102" s="36"/>
-      <c r="M102" s="36"/>
-      <c r="N102" s="37"/>
-    </row>
-    <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="48">
-        <v>1.0</v>
-      </c>
-      <c r="B103" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="50" t="s">
+      <c r="N104" s="40"/>
+    </row>
+    <row r="105" ht="14.25" customHeight="1">
+      <c r="A105" s="51">
+        <v>3.0</v>
+      </c>
+      <c r="B105" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C105" s="6"/>
+      <c r="D105" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E105" s="6"/>
+      <c r="G105" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E103" s="6"/>
-      <c r="G103" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H103" s="37"/>
-      <c r="I103" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="J103" s="37"/>
-      <c r="K103" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="L103" s="37"/>
-      <c r="M103" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="N103" s="37"/>
-    </row>
-    <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="48">
-        <v>2.0</v>
-      </c>
-      <c r="B104" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="54" t="s">
+      <c r="H105" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I105" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="J105" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="K105" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="L105" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="M105" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="N105" s="50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" ht="14.25" customHeight="1">
+      <c r="A106" s="51">
+        <v>4.0</v>
+      </c>
+      <c r="B106" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E106" s="6"/>
+      <c r="G106" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H106" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I106" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J106" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K106" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L106" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M106" s="54"/>
+      <c r="N106" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25" customHeight="1">
+      <c r="A107" s="59">
+        <v>5.0</v>
+      </c>
+      <c r="B107" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="6"/>
+      <c r="G107" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H107" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I107" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J107" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K107" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L107" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M107" s="54"/>
+      <c r="N107" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="A108" s="59">
+        <v>6.0</v>
+      </c>
+      <c r="B108" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="E108" s="6"/>
+      <c r="G108" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H108" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I108" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J108" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K108" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L108" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="M108" s="54"/>
+      <c r="N108" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="109" ht="14.25" customHeight="1">
+      <c r="A109" s="59">
+        <v>7.0</v>
+      </c>
+      <c r="B109" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" s="6"/>
+      <c r="D109" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E109" s="6"/>
+      <c r="G109" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H109" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I109" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J109" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K109" s="58"/>
+      <c r="L109" s="25"/>
+      <c r="M109" s="58"/>
+      <c r="N109" s="25"/>
+    </row>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="A110" s="59">
+        <v>8.0</v>
+      </c>
+      <c r="B110" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C110" s="6"/>
+      <c r="D110" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E110" s="6"/>
+      <c r="G110" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H110" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I110" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J110" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K110" s="58"/>
+      <c r="L110" s="25"/>
+      <c r="M110" s="58"/>
+      <c r="N110" s="25"/>
+    </row>
+    <row r="111" ht="14.25" customHeight="1">
+      <c r="A111" s="59">
+        <v>9.0</v>
+      </c>
+      <c r="B111" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C111" s="6"/>
+      <c r="D111" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E111" s="6"/>
+      <c r="G111" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H111" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I111" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J111" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E104" s="6"/>
-      <c r="G104" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H104" s="37"/>
-      <c r="I104" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="J104" s="37"/>
-      <c r="K104" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="L104" s="37"/>
-      <c r="M104" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="N104" s="37"/>
-    </row>
-    <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="48">
-        <v>3.0</v>
-      </c>
-      <c r="B105" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E105" s="6"/>
-      <c r="G105" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H105" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="I105" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J105" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="K105" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="L105" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="M105" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="N105" s="47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="48">
-        <v>4.0</v>
-      </c>
-      <c r="B106" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="E106" s="6"/>
-      <c r="G106" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H106" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I106" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J106" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K106" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L106" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M106" s="51"/>
-      <c r="N106" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="56">
-        <v>5.0</v>
-      </c>
-      <c r="B107" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C107" s="6"/>
-      <c r="D107" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="E107" s="6"/>
-      <c r="G107" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H107" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I107" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J107" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K107" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L107" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M107" s="51"/>
-      <c r="N107" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="56">
-        <v>6.0</v>
-      </c>
-      <c r="B108" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C108" s="6"/>
-      <c r="D108" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="E108" s="6"/>
-      <c r="G108" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H108" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I108" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J108" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K108" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L108" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M108" s="51"/>
-      <c r="N108" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="56">
-        <v>7.0</v>
-      </c>
-      <c r="B109" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E109" s="6"/>
-      <c r="G109" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H109" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I109" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J109" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K109" s="55"/>
-      <c r="L109" s="25"/>
-      <c r="M109" s="55"/>
-      <c r="N109" s="25"/>
-    </row>
-    <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="56">
-        <v>8.0</v>
-      </c>
-      <c r="B110" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="C110" s="6"/>
-      <c r="D110" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E110" s="6"/>
-      <c r="G110" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H110" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I110" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J110" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="K110" s="55"/>
-      <c r="L110" s="25"/>
-      <c r="M110" s="55"/>
-      <c r="N110" s="25"/>
-    </row>
-    <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="56">
-        <v>9.0</v>
-      </c>
-      <c r="B111" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E111" s="6"/>
-      <c r="G111" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H111" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I111" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J111" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="K111" s="55"/>
+      <c r="K111" s="58"/>
       <c r="L111" s="25"/>
-      <c r="M111" s="55"/>
+      <c r="M111" s="58"/>
       <c r="N111" s="25"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="56">
+      <c r="A112" s="59">
         <v>10.0</v>
       </c>
-      <c r="B112" s="54" t="s">
-        <v>97</v>
+      <c r="B112" s="57" t="s">
+        <v>103</v>
       </c>
       <c r="C112" s="6"/>
-      <c r="D112" s="54" t="s">
-        <v>71</v>
+      <c r="D112" s="57" t="s">
+        <v>74</v>
       </c>
       <c r="E112" s="6"/>
-      <c r="G112" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H112" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I112" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J112" s="52" t="s">
-        <v>51</v>
+      <c r="G112" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H112" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I112" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J112" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="56">
+      <c r="A113" s="59">
         <v>11.0</v>
       </c>
-      <c r="B113" s="54" t="s">
-        <v>98</v>
+      <c r="B113" s="57" t="s">
+        <v>104</v>
       </c>
       <c r="C113" s="6"/>
-      <c r="D113" s="54" t="s">
-        <v>73</v>
+      <c r="D113" s="57" t="s">
+        <v>76</v>
       </c>
       <c r="E113" s="6"/>
-      <c r="G113" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H113" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I113" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J113" s="52" t="s">
-        <v>51</v>
+      <c r="G113" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H113" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I113" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J113" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="56">
+      <c r="A114" s="59">
         <v>12.0</v>
       </c>
-      <c r="B114" s="54" t="s">
-        <v>99</v>
+      <c r="B114" s="57" t="s">
+        <v>77</v>
       </c>
       <c r="C114" s="6"/>
-      <c r="D114" s="54" t="s">
-        <v>75</v>
+      <c r="D114" s="57" t="s">
+        <v>123</v>
       </c>
       <c r="E114" s="6"/>
-      <c r="G114" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H114" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I114" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J114" s="52" t="s">
-        <v>51</v>
+      <c r="G114" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H114" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I114" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J114" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="56">
+      <c r="A115" s="59">
         <v>13.0</v>
       </c>
-      <c r="B115" s="54" t="s">
-        <v>76</v>
+      <c r="B115" s="57" t="s">
+        <v>105</v>
       </c>
       <c r="C115" s="6"/>
-      <c r="D115" s="54" t="s">
-        <v>100</v>
+      <c r="D115" s="57" t="s">
+        <v>80</v>
       </c>
       <c r="E115" s="6"/>
-      <c r="G115" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H115" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I115" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J115" s="52" t="s">
-        <v>51</v>
+      <c r="G115" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H115" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I115" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J115" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="G116" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H116" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I116" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J116" s="52" t="s">
-        <v>51</v>
+      <c r="A116" s="59">
+        <v>14.0</v>
+      </c>
+      <c r="B116" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="D116" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="E116" s="6"/>
+      <c r="G116" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H116" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I116" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J116" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="G117" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H117" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I117" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J117" s="52" t="s">
-        <v>51</v>
+      <c r="G117" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H117" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I117" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J117" s="55" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="G118" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="H118" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I118" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J118" s="53" t="s">
-        <v>52</v>
+      <c r="G118" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H118" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I118" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J118" s="56" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1"/>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="G120" s="57" t="s">
-        <v>78</v>
+      <c r="G120" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="H120" s="6"/>
-      <c r="I120" s="57" t="s">
-        <v>78</v>
+      <c r="I120" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="J120" s="6"/>
-      <c r="K120" s="57" t="s">
-        <v>78</v>
+      <c r="K120" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="L120" s="6"/>
-      <c r="M120" s="57" t="s">
-        <v>78</v>
+      <c r="M120" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="N120" s="6"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="G121" s="58"/>
+      <c r="G121" s="61"/>
       <c r="H121" s="6"/>
-      <c r="I121" s="59" t="s">
-        <v>101</v>
+      <c r="I121" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="J121" s="6"/>
-      <c r="K121" s="58"/>
+      <c r="K121" s="61"/>
       <c r="L121" s="6"/>
-      <c r="M121" s="58"/>
+      <c r="M121" s="61"/>
       <c r="N121" s="6"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="G122" s="58"/>
+      <c r="G122" s="61"/>
       <c r="H122" s="6"/>
-      <c r="I122" s="59" t="s">
-        <v>102</v>
+      <c r="I122" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="J122" s="6"/>
-      <c r="K122" s="58"/>
+      <c r="K122" s="61"/>
       <c r="L122" s="6"/>
-      <c r="M122" s="58"/>
+      <c r="M122" s="61"/>
       <c r="N122" s="6"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="G123" s="58"/>
+      <c r="G123" s="61"/>
       <c r="H123" s="6"/>
-      <c r="I123" s="58"/>
+      <c r="I123" s="61"/>
       <c r="J123" s="6"/>
-      <c r="K123" s="58"/>
+      <c r="K123" s="61"/>
       <c r="L123" s="6"/>
-      <c r="M123" s="58"/>
+      <c r="M123" s="61"/>
       <c r="N123" s="6"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="G124" s="58"/>
+      <c r="G124" s="61"/>
       <c r="H124" s="6"/>
-      <c r="I124" s="58"/>
+      <c r="I124" s="61"/>
       <c r="J124" s="6"/>
-      <c r="K124" s="58"/>
+      <c r="K124" s="61"/>
       <c r="L124" s="6"/>
-      <c r="M124" s="58"/>
+      <c r="M124" s="61"/>
       <c r="N124" s="6"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="G125" s="58"/>
+      <c r="G125" s="61"/>
       <c r="H125" s="6"/>
-      <c r="I125" s="58"/>
+      <c r="I125" s="61"/>
       <c r="J125" s="6"/>
-      <c r="K125" s="58"/>
+      <c r="K125" s="61"/>
       <c r="L125" s="6"/>
-      <c r="M125" s="58"/>
+      <c r="M125" s="61"/>
       <c r="N125" s="6"/>
     </row>
     <row r="126" ht="14.25" customHeight="1"/>
@@ -4176,7 +4309,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="190">
+  <mergeCells count="199">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:E21"/>
@@ -4184,6 +4317,7 @@
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:J23"/>
@@ -4199,8 +4333,9 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
@@ -4215,14 +4350,15 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="M40:N40"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="K40:L40"/>
     <mergeCell ref="G41:H41"/>
@@ -4246,6 +4382,7 @@
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="G63:N63"/>
+    <mergeCell ref="D55:E55"/>
     <mergeCell ref="G64:H64"/>
     <mergeCell ref="G65:H65"/>
     <mergeCell ref="I65:J65"/>
@@ -4267,8 +4404,9 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
     <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="B70:C70"/>
@@ -4278,11 +4416,12 @@
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
     <mergeCell ref="G82:H82"/>
     <mergeCell ref="I81:J81"/>
     <mergeCell ref="G81:H81"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D75:E75"/>
     <mergeCell ref="M83:N83"/>
     <mergeCell ref="M84:N84"/>
     <mergeCell ref="M85:N85"/>
@@ -4325,13 +4464,14 @@
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="G104:H104"/>
     <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D94:E94"/>
     <mergeCell ref="G86:H86"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="B109:C109"/>
     <mergeCell ref="B111:C111"/>
     <mergeCell ref="B110:C110"/>
     <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D110:E110"/>
     <mergeCell ref="D111:E111"/>
     <mergeCell ref="I82:J82"/>
     <mergeCell ref="I84:J84"/>
@@ -4359,14 +4499,16 @@
     <mergeCell ref="D112:E112"/>
     <mergeCell ref="D113:E113"/>
     <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
     <mergeCell ref="D114:E114"/>
     <mergeCell ref="B105:C105"/>
     <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B114:C114"/>
     <mergeCell ref="B108:C108"/>
     <mergeCell ref="B113:C113"/>
     <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B114:C114"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B25"/>

</xml_diff>